<commit_message>
819541 Updated for IOC Exit
</commit_message>
<xml_diff>
--- a/Test/Build 4/TAS eBill Defect Log IB_2.0_592.xlsx
+++ b/Test/Build 4/TAS eBill Defect Log IB_2.0_592.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vhaispbalchj\Documents\eBilling Docs\Build 3&amp;4\Docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="384" yWindow="-12" windowWidth="22668" windowHeight="7848" activeTab="2"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="186">
   <si>
     <t>Department of Veterans Affairs</t>
   </si>
@@ -136,9 +141,6 @@
   </si>
   <si>
     <t>US2488: Update Reports - Form Type J430D</t>
-  </si>
-  <si>
-    <t>2 - Low</t>
   </si>
   <si>
     <t>DE316</t>
@@ -400,9 +402,6 @@
     <t>DE374</t>
   </si>
   <si>
-    <t>4 - Medium</t>
-  </si>
-  <si>
     <t>CIT -  Transmission Method - US1108</t>
   </si>
   <si>
@@ -499,8 +498,122 @@
     <t>CIT -  Provider ID Maintenance Main Menu Spelling Error</t>
   </si>
   <si>
+    <t>December 2017</t>
+  </si>
+  <si>
+    <t>TS27: Regression VA Provider’s Own ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9/6/2017 Found in B*2.0*592_T1 </t>
+  </si>
+  <si>
+    <t>9/21/2017 Fixed in  IB*2.0*592_T2</t>
+  </si>
+  <si>
+    <t>11/9/2017 Found in IB*2.0*592_T6</t>
+  </si>
+  <si>
+    <t>11/9/2017 Found in IB*2.0*592_T7</t>
+  </si>
+  <si>
+    <t>11/13/2017 Found in IB*2.0*592_T7</t>
+  </si>
+  <si>
+    <t>11/30/2017 Found in IB*20*592_T9</t>
+  </si>
+  <si>
+    <t>12/5/2017 Fixed in IB*20*592_T10</t>
+  </si>
+  <si>
+    <t>9/19/2017 Fixed in IB*2.0*592_T2</t>
+  </si>
+  <si>
+    <t>9/20/2017 Fixed in IB*2.0*592_T2</t>
+  </si>
+  <si>
+    <t>9/26/2017 Fixed in IB*2.0*592_T3</t>
+  </si>
+  <si>
+    <t>9/26/2017 Fixed in  IB*2.0*592_T3</t>
+  </si>
+  <si>
+    <t>10/24/2017 Fixed in IB*2.0*592_T5</t>
+  </si>
+  <si>
+    <t>10/18/2017 Fixed in IB*2.0*592_T4</t>
+  </si>
+  <si>
+    <t>11/13/2017 Fixed in IB*20*592_T7</t>
+  </si>
+  <si>
+    <t>9/20/2017 Fixed In IB*2.0*592_T2</t>
+  </si>
+  <si>
+    <t>11/1/2017 Found in B*2.0*592_T6</t>
+  </si>
+  <si>
+    <t>IOC - A tooth number showing up from a previous claim</t>
+  </si>
+  <si>
+    <t>DE832</t>
+  </si>
+  <si>
+    <t>6/26/2018 Found in IB*20*592_T15</t>
+  </si>
+  <si>
+    <t>7/9/2018 Fixed in IB*20*592_T17</t>
+  </si>
+  <si>
+    <t>IOC - ‘Mismatched’ procedure lines message appearing on the TPJI screen for EOB display</t>
+  </si>
+  <si>
+    <t>DE845</t>
+  </si>
+  <si>
+    <t>TC1621: CIT eBilling TS21 EDI Claim Status Report_Dental US2488</t>
+  </si>
+  <si>
+    <t>7/10/2018 Found in IB*20*592_T17</t>
+  </si>
+  <si>
+    <t>7/17/2018 Fixed in IB*20*592_T18</t>
+  </si>
+  <si>
+    <t>DE893</t>
+  </si>
+  <si>
+    <t>IOC - IF Dental Claims are off - no claims can be created</t>
+  </si>
+  <si>
+    <t>7/31/2018 Found in IB*20*592_T18</t>
+  </si>
+  <si>
+    <t>8/7/2018 Fixed in IB*20*592_T19</t>
+  </si>
+  <si>
+    <t>DE894</t>
+  </si>
+  <si>
+    <t>IOC - Tooth number overwrite</t>
+  </si>
+  <si>
+    <t>8/1/2018 Found in IB*20*592_T18</t>
+  </si>
+  <si>
+    <t>4 - Low</t>
+  </si>
+  <si>
+    <t>September 2018</t>
+  </si>
+  <si>
+    <t>Updated with final build T20 test defects and test results</t>
+  </si>
+  <si>
+    <t>Updated with final build test defects and test results</t>
+  </si>
+  <si>
     <r>
-      <t>Version 3.0</t>
+      <t>Version 4.0</t>
     </r>
     <r>
       <rPr>
@@ -513,68 +626,11 @@
       <t xml:space="preserve">               </t>
     </r>
   </si>
-  <si>
-    <t>December 2017</t>
-  </si>
-  <si>
-    <t>Updated with final build test defect test results</t>
-  </si>
-  <si>
-    <t>TS27: Regression VA Provider’s Own ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9/6/2017 Found in B*2.0*592_T1 </t>
-  </si>
-  <si>
-    <t>9/21/2017 Fixed in  IB*2.0*592_T2</t>
-  </si>
-  <si>
-    <t>11/9/2017 Found in IB*2.0*592_T6</t>
-  </si>
-  <si>
-    <t>11/9/2017 Found in IB*2.0*592_T7</t>
-  </si>
-  <si>
-    <t>11/13/2017 Found in IB*2.0*592_T7</t>
-  </si>
-  <si>
-    <t>11/30/2017 Found in IB*20*592_T9</t>
-  </si>
-  <si>
-    <t>12/5/2017 Fixed in IB*20*592_T10</t>
-  </si>
-  <si>
-    <t>9/19/2017 Fixed in IB*2.0*592_T2</t>
-  </si>
-  <si>
-    <t>9/20/2017 Fixed in IB*2.0*592_T2</t>
-  </si>
-  <si>
-    <t>9/26/2017 Fixed in IB*2.0*592_T3</t>
-  </si>
-  <si>
-    <t>9/26/2017 Fixed in  IB*2.0*592_T3</t>
-  </si>
-  <si>
-    <t>10/24/2017 Fixed in IB*2.0*592_T5</t>
-  </si>
-  <si>
-    <t>10/18/2017 Fixed in IB*2.0*592_T4</t>
-  </si>
-  <si>
-    <t>11/13/2017 Fixed in IB*20*592_T7</t>
-  </si>
-  <si>
-    <t>9/20/2017 Fixed In IB*2.0*592_T2</t>
-  </si>
-  <si>
-    <t>11/1/2017 Found in B*2.0*592_T6</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -1275,7 +1331,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1">
@@ -1401,9 +1457,6 @@
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1729,6 +1782,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1750,7 +1806,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1831,7 +1893,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1864,9 +1926,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1899,6 +1978,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2077,8 +2173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:H34"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:H23"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2088,43 +2184,43 @@
     <col min="4" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A5" s="52" t="s">
+    <row r="5" spans="1:8" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="A5" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="52"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
-    </row>
-    <row r="6" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B5" s="51"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="51"/>
+    </row>
+    <row r="6" spans="1:8" ht="22.8" x14ac:dyDescent="0.4">
       <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:8" ht="118.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="53" t="s">
-        <v>66</v>
-      </c>
-      <c r="B7" s="54"/>
-      <c r="C7" s="54"/>
-      <c r="D7" s="54"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="54"/>
-      <c r="G7" s="54"/>
-      <c r="H7" s="54"/>
-    </row>
-    <row r="8" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A7" s="52" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" s="53"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
+    </row>
+    <row r="8" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C11" s="3"/>
     </row>
     <row r="12" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -2148,26 +2244,26 @@
     <row r="18" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C18" s="3"/>
     </row>
-    <row r="20" spans="1:8" ht="13.95" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:8" ht="13.95" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C21" s="4"/>
     </row>
     <row r="22" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C22" s="4"/>
     </row>
     <row r="23" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="55" t="s">
-        <v>150</v>
-      </c>
-      <c r="B23" s="55"/>
-      <c r="C23" s="55"/>
-      <c r="D23" s="55"/>
-      <c r="E23" s="55"/>
-      <c r="F23" s="55"/>
-      <c r="G23" s="55"/>
-      <c r="H23" s="55"/>
+      <c r="A23" s="54" t="s">
+        <v>182</v>
+      </c>
+      <c r="B23" s="54"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="54"/>
+      <c r="H23" s="54"/>
     </row>
     <row r="24" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B24" s="3"/>
@@ -2178,16 +2274,16 @@
       <c r="C25" s="5"/>
     </row>
     <row r="26" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A26" s="56" t="s">
-        <v>149</v>
-      </c>
-      <c r="B26" s="56"/>
-      <c r="C26" s="56"/>
-      <c r="D26" s="56"/>
-      <c r="E26" s="56"/>
-      <c r="F26" s="56"/>
-      <c r="G26" s="56"/>
-      <c r="H26" s="56"/>
+      <c r="A26" s="55" t="s">
+        <v>185</v>
+      </c>
+      <c r="B26" s="55"/>
+      <c r="C26" s="55"/>
+      <c r="D26" s="55"/>
+      <c r="E26" s="55"/>
+      <c r="F26" s="55"/>
+      <c r="G26" s="55"/>
+      <c r="H26" s="55"/>
     </row>
     <row r="29" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="6"/>
@@ -2225,7 +2321,7 @@
   <dimension ref="A2:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D9:D10"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2238,14 +2334,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-    </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+    </row>
+    <row r="3" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>2</v>
       </c>
@@ -2261,13 +2357,13 @@
     </row>
     <row r="4" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A4" s="37" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B4" s="18">
         <v>1</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D4" s="17" t="s">
         <v>9</v>
@@ -2275,13 +2371,13 @@
     </row>
     <row r="5" spans="1:4" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B5" s="16">
         <v>2</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D5" s="17" t="s">
         <v>9</v>
@@ -2289,23 +2385,31 @@
     </row>
     <row r="6" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B6" s="16">
         <v>3</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>151</v>
+        <v>184</v>
       </c>
       <c r="D6" s="17" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="17"/>
+    <row r="7" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="B7" s="19">
+        <v>4</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A8" s="37"/>
@@ -2378,10 +2482,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A44" sqref="A44:XFD44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -2399,7 +2503,7 @@
     <col min="11" max="16384" width="10.6640625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>7</v>
       </c>
@@ -2432,7 +2536,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="50" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="21" t="s">
@@ -2445,24 +2549,24 @@
         <v>8</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G2" s="21" t="s">
         <v>20</v>
       </c>
       <c r="H2" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="J2" s="9"/>
     </row>
     <row r="3" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="50" t="s">
         <v>21</v>
       </c>
       <c r="B3" s="21" t="s">
@@ -2475,24 +2579,24 @@
         <v>8</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G3" s="21" t="s">
         <v>23</v>
       </c>
       <c r="H3" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="J3" s="11"/>
     </row>
     <row r="4" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="50" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="21" t="s">
@@ -2505,91 +2609,91 @@
         <v>8</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F4" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G4" s="21" t="s">
         <v>23</v>
       </c>
       <c r="H4" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="J4" s="11"/>
     </row>
     <row r="5" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="50" t="s">
         <v>26</v>
       </c>
       <c r="B5" s="21" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D5" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G5" s="21" t="s">
         <v>20</v>
       </c>
       <c r="H5" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="J5" s="11"/>
     </row>
     <row r="6" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="51" t="s">
+      <c r="A6" s="50" t="s">
         <v>27</v>
       </c>
       <c r="B6" s="21" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D6" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G6" s="21" t="s">
         <v>20</v>
       </c>
       <c r="H6" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="J6" s="11"/>
     </row>
     <row r="7" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="50" t="s">
         <v>28</v>
       </c>
       <c r="B7" s="21" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D7" s="21" t="s">
         <v>8</v>
@@ -2598,21 +2702,21 @@
         <v>17</v>
       </c>
       <c r="F7" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G7" s="21" t="s">
         <v>20</v>
       </c>
       <c r="H7" s="21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J7" s="11"/>
     </row>
     <row r="8" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="51" t="s">
+      <c r="A8" s="50" t="s">
         <v>29</v>
       </c>
       <c r="B8" s="21" t="s">
@@ -2625,24 +2729,24 @@
         <v>8</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G8" s="21" t="s">
         <v>20</v>
       </c>
       <c r="H8" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="J8" s="11"/>
     </row>
     <row r="9" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="51" t="s">
+      <c r="A9" s="50" t="s">
         <v>31</v>
       </c>
       <c r="B9" s="21" t="s">
@@ -2655,24 +2759,24 @@
         <v>8</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F9" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G9" s="21" t="s">
         <v>23</v>
       </c>
       <c r="H9" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="J9" s="11"/>
     </row>
     <row r="10" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="51" t="s">
+      <c r="A10" s="50" t="s">
         <v>33</v>
       </c>
       <c r="B10" s="21" t="s">
@@ -2685,54 +2789,54 @@
         <v>35</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="G10" s="21" t="s">
         <v>20</v>
       </c>
       <c r="H10" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I10" s="13" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="J10" s="11"/>
     </row>
     <row r="11" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="51" t="s">
+      <c r="A11" s="50" t="s">
         <v>36</v>
       </c>
       <c r="B11" s="21" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D11" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G11" s="21" t="s">
         <v>20</v>
       </c>
       <c r="H11" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="J11" s="11"/>
     </row>
     <row r="12" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="51" t="s">
+      <c r="A12" s="50" t="s">
         <v>37</v>
       </c>
       <c r="B12" s="21" t="s">
@@ -2742,869 +2846,965 @@
         <v>38</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>40</v>
+        <v>181</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G12" s="21" t="s">
         <v>39</v>
       </c>
       <c r="H12" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="J12" s="11"/>
+    </row>
+    <row r="13" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="I12" s="13" t="s">
-        <v>162</v>
-      </c>
-      <c r="J12" s="11"/>
-    </row>
-    <row r="13" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="51" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="21" t="s">
+      <c r="I13" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="J13" s="11"/>
+    </row>
+    <row r="14" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="F13" s="21" t="s">
+      <c r="H14" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="J14" s="11"/>
+    </row>
+    <row r="15" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="G13" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="H13" s="21" t="s">
+      <c r="G15" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="H15" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="I13" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="J13" s="11"/>
-    </row>
-    <row r="14" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="51" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="F14" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="G14" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="H14" s="21" t="s">
+      <c r="I15" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="J15" s="11"/>
+    </row>
+    <row r="16" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="50" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="H16" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="I14" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="J14" s="11"/>
-    </row>
-    <row r="15" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="51" t="s">
-        <v>45</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="D15" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="F15" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="G15" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="H15" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="I15" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="J15" s="11"/>
-    </row>
-    <row r="16" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="51" t="s">
-        <v>65</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="F16" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="G16" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="H16" s="21" t="s">
-        <v>64</v>
-      </c>
       <c r="I16" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J16" s="11"/>
     </row>
     <row r="17" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A17" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="B17" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>69</v>
-      </c>
       <c r="D17" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G17" s="12" t="s">
         <v>23</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I17" s="11" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="J17" s="11"/>
     </row>
     <row r="18" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A18" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B18" s="22" t="s">
         <v>17</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D18" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G18" s="21" t="s">
         <v>20</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J18" s="11"/>
     </row>
     <row r="19" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A19" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B19" s="22" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="F19" s="12" t="s">
         <v>71</v>
-      </c>
-      <c r="D19" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>72</v>
       </c>
       <c r="G19" s="21" t="s">
         <v>20</v>
       </c>
       <c r="H19" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J19" s="11"/>
     </row>
     <row r="20" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A20" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="B20" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="24" t="s">
-        <v>83</v>
-      </c>
       <c r="D20" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E20" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G20" s="21" t="s">
         <v>20</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J20" s="11"/>
     </row>
     <row r="21" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A21" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="B21" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="12" t="s">
+      <c r="D21" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="F21" s="12" t="s">
         <v>86</v>
-      </c>
-      <c r="D21" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>87</v>
       </c>
       <c r="G21" s="21" t="s">
         <v>20</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I21" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J21" s="11"/>
     </row>
     <row r="22" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A22" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="F22" s="12" t="s">
         <v>88</v>
-      </c>
-      <c r="B22" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="D22" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>89</v>
       </c>
       <c r="G22" s="21" t="s">
         <v>20</v>
       </c>
       <c r="H22" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I22" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J22" s="11"/>
     </row>
     <row r="23" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="51" t="s">
+      <c r="A23" s="50" t="s">
+        <v>92</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="B23" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="C23" s="21" t="s">
+      <c r="D23" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23" s="21" t="s">
         <v>94</v>
-      </c>
-      <c r="D23" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="F23" s="21" t="s">
-        <v>95</v>
       </c>
       <c r="G23" s="21" t="s">
         <v>23</v>
       </c>
       <c r="H23" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I23" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J23" s="11"/>
     </row>
     <row r="24" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="51" t="s">
+      <c r="A24" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="B24" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" s="21" t="s">
-        <v>92</v>
-      </c>
       <c r="D24" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F24" s="21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G24" s="21" t="s">
         <v>23</v>
       </c>
       <c r="H24" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I24" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J24" s="11"/>
     </row>
     <row r="25" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A25" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="F25" s="21" t="s">
         <v>98</v>
-      </c>
-      <c r="B25" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="D25" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="F25" s="21" t="s">
-        <v>99</v>
       </c>
       <c r="G25" s="21" t="s">
         <v>20</v>
       </c>
       <c r="H25" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I25" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J25" s="11"/>
     </row>
     <row r="26" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A26" s="22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B26" s="22" t="s">
         <v>17</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D26" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F26" s="21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G26" s="21" t="s">
         <v>20</v>
       </c>
       <c r="H26" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I26" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J26" s="11"/>
     </row>
     <row r="27" spans="1:10" s="43" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A27" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="B27" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="B27" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27" s="21" t="s">
+      <c r="D27" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="F27" s="21" t="s">
         <v>103</v>
-      </c>
-      <c r="D27" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="F27" s="21" t="s">
-        <v>104</v>
       </c>
       <c r="G27" s="21" t="s">
         <v>20</v>
       </c>
       <c r="H27" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I27" s="13" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="J27" s="42"/>
     </row>
     <row r="28" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A28" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B28" s="22" t="s">
         <v>17</v>
       </c>
       <c r="C28" s="44" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D28" s="36" t="s">
         <v>8</v>
       </c>
       <c r="E28" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F28" s="21" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="G28" s="21" t="s">
         <v>20</v>
       </c>
       <c r="H28" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I28" s="13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="J28" s="11"/>
     </row>
     <row r="29" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A29" s="22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B29" s="22" t="s">
         <v>17</v>
       </c>
       <c r="C29" s="44" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D29" s="36" t="s">
         <v>8</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F29" s="21" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="G29" s="21" t="s">
         <v>23</v>
       </c>
       <c r="H29" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I29" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="J29" s="11"/>
     </row>
     <row r="30" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A30" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="B30" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="D30" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="F30" s="21" t="s">
         <v>113</v>
-      </c>
-      <c r="B30" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C30" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="D30" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="E30" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="F30" s="21" t="s">
-        <v>114</v>
       </c>
       <c r="G30" s="21" t="s">
         <v>20</v>
       </c>
       <c r="H30" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I30" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="J30" s="11"/>
     </row>
     <row r="31" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A31" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="B31" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="B31" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C31" s="22" t="s">
-        <v>117</v>
-      </c>
       <c r="D31" s="36" t="s">
-        <v>116</v>
+        <v>8</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F31" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G31" s="21" t="s">
         <v>20</v>
       </c>
       <c r="H31" s="21" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I31" s="13" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J31" s="11"/>
     </row>
     <row r="32" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A32" s="22" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B32" s="22" t="s">
         <v>17</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D32" s="36" t="s">
-        <v>116</v>
+        <v>8</v>
       </c>
       <c r="E32" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F32" s="21" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="G32" s="21" t="s">
         <v>23</v>
       </c>
       <c r="H32" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I32" s="13" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="J32" s="11"/>
     </row>
     <row r="33" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A33" s="22" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B33" s="22" t="s">
         <v>17</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D33" s="36" t="s">
-        <v>116</v>
+        <v>8</v>
       </c>
       <c r="E33" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F33" s="21" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="G33" s="21" t="s">
         <v>23</v>
       </c>
       <c r="H33" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I33" s="13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="J33" s="11"/>
     </row>
     <row r="34" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A34" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="B34" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" s="45" t="s">
+        <v>125</v>
+      </c>
+      <c r="D34" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="F34" s="46" t="s">
+        <v>152</v>
+      </c>
+      <c r="G34" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="H34" s="46" t="s">
+        <v>56</v>
+      </c>
+      <c r="I34" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="J34" s="47"/>
+    </row>
+    <row r="35" spans="1:10" s="48" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="B34" s="45" t="s">
-        <v>17</v>
-      </c>
-      <c r="C34" s="45" t="s">
-        <v>127</v>
-      </c>
-      <c r="D34" s="46" t="s">
-        <v>116</v>
-      </c>
-      <c r="E34" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="F34" s="47" t="s">
-        <v>156</v>
-      </c>
-      <c r="G34" s="47" t="s">
-        <v>23</v>
-      </c>
-      <c r="H34" s="47" t="s">
-        <v>57</v>
-      </c>
-      <c r="I34" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="J34" s="48"/>
-    </row>
-    <row r="35" spans="1:10" s="49" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="22" t="s">
+      <c r="B35" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="B35" s="45" t="s">
-        <v>17</v>
-      </c>
-      <c r="C35" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="D35" s="46" t="s">
-        <v>116</v>
+      <c r="D35" s="36" t="s">
+        <v>8</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="F35" s="47" t="s">
-        <v>157</v>
+        <v>66</v>
+      </c>
+      <c r="F35" s="46" t="s">
+        <v>153</v>
       </c>
       <c r="G35" s="21" t="s">
         <v>39</v>
       </c>
       <c r="H35" s="21" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="I35" s="13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="J35" s="11"/>
     </row>
-    <row r="36" spans="1:10" s="49" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" s="48" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A36" s="22" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B36" s="45" t="s">
         <v>17</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>132</v>
-      </c>
-      <c r="D36" s="46" t="s">
-        <v>116</v>
+        <v>130</v>
+      </c>
+      <c r="D36" s="36" t="s">
+        <v>8</v>
       </c>
       <c r="E36" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="F36" s="47" t="s">
-        <v>157</v>
+        <v>66</v>
+      </c>
+      <c r="F36" s="46" t="s">
+        <v>153</v>
       </c>
       <c r="G36" s="21" t="s">
         <v>20</v>
       </c>
       <c r="H36" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I36" s="13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="J36" s="11"/>
     </row>
-    <row r="37" spans="1:10" s="49" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" s="48" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A37" s="22" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B37" s="45" t="s">
         <v>17</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>143</v>
-      </c>
-      <c r="D37" s="46" t="s">
-        <v>116</v>
+        <v>141</v>
+      </c>
+      <c r="D37" s="36" t="s">
+        <v>8</v>
       </c>
       <c r="E37" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F37" s="13" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G37" s="21" t="s">
         <v>20</v>
       </c>
       <c r="H37" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="I37" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="J37" s="11"/>
+    </row>
+    <row r="38" spans="1:10" s="48" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="B38" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="I37" s="13" t="s">
+      <c r="D38" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="F38" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="G38" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="H38" s="49" t="s">
+        <v>137</v>
+      </c>
+      <c r="I38" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="J38" s="11"/>
+    </row>
+    <row r="39" spans="1:10" s="48" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="B39" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" s="22" t="s">
         <v>146</v>
       </c>
-      <c r="J37" s="11"/>
-    </row>
-    <row r="38" spans="1:10" s="49" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="22" t="s">
-        <v>141</v>
-      </c>
-      <c r="B38" s="45" t="s">
-        <v>17</v>
-      </c>
-      <c r="C38" s="22" t="s">
-        <v>140</v>
-      </c>
-      <c r="D38" s="46" t="s">
-        <v>116</v>
-      </c>
-      <c r="E38" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="F38" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="G38" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="H38" s="50" t="s">
-        <v>139</v>
-      </c>
-      <c r="I38" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="J38" s="11"/>
-    </row>
-    <row r="39" spans="1:10" s="49" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="22" t="s">
+      <c r="D39" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="G39" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="B39" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C39" s="22" t="s">
+      <c r="H39" s="50" t="s">
         <v>148</v>
       </c>
-      <c r="D39" s="46" t="s">
-        <v>116</v>
-      </c>
-      <c r="E39" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="F39" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="G39" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="H39" s="51" t="s">
-        <v>152</v>
-      </c>
       <c r="I39" s="13" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="J39" s="11"/>
     </row>
-    <row r="40" spans="1:10" s="49" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="12"/>
-      <c r="B40" s="22"/>
-      <c r="C40" s="22"/>
-      <c r="D40" s="21"/>
-      <c r="E40" s="21"/>
-      <c r="F40" s="21"/>
-      <c r="G40" s="21"/>
-      <c r="H40" s="21"/>
-      <c r="I40" s="11"/>
+    <row r="40" spans="1:10" s="48" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="B40" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="D40" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="F40" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="G40" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="H40" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="I40" s="13" t="s">
+        <v>168</v>
+      </c>
       <c r="J40" s="11"/>
     </row>
-    <row r="41" spans="1:10" s="49" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="12"/>
-      <c r="B41" s="22"/>
-      <c r="C41" s="22"/>
-      <c r="D41" s="21"/>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21"/>
-      <c r="G41" s="21"/>
-      <c r="H41" s="21"/>
-      <c r="I41" s="11"/>
+    <row r="41" spans="1:10" s="48" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A41" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="B41" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="D41" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="F41" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="G41" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="H41" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="I41" s="13" t="s">
+        <v>173</v>
+      </c>
       <c r="J41" s="11"/>
     </row>
-    <row r="42" spans="1:10" s="49" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="11"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11"/>
-      <c r="I42" s="11"/>
+    <row r="42" spans="1:10" s="48" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A42" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="B42" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" s="22" t="s">
+        <v>175</v>
+      </c>
+      <c r="D42" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="F42" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="G42" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="H42" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="I42" s="13" t="s">
+        <v>177</v>
+      </c>
       <c r="J42" s="11"/>
+    </row>
+    <row r="43" spans="1:10" s="48" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A43" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="B43" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C43" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="D43" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="F43" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="G43" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="H43" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="I43" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="J43" s="11"/>
+    </row>
+    <row r="44" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="11"/>
+      <c r="J44" s="11"/>
     </row>
   </sheetData>
   <sortState ref="A2:H13">

</xml_diff>